<commit_message>
Starting to set up models
</commit_message>
<xml_diff>
--- a/ats_project-tables.xlsx
+++ b/ats_project-tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>title</t>
   </si>
@@ -30,30 +30,18 @@
     <t>description</t>
   </si>
   <si>
-    <t>text_area</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
     <t>city</t>
   </si>
   <si>
-    <t>zip_code</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>integer</t>
   </si>
   <si>
-    <t>Job:jobs</t>
-  </si>
-  <si>
-    <t>workflow_id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -81,12 +69,6 @@
     <t>emails</t>
   </si>
   <si>
-    <t>WorkflowStatus:workflow_status</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -135,17 +117,98 @@
     <t>Hired elsewhere</t>
   </si>
   <si>
-    <t>Applicant:applicants</t>
-  </si>
-  <si>
     <t>resume</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>Table: jobs  Class: Job</t>
+  </si>
+  <si>
+    <t>Table: applicants  class: Applicant</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>applicant_id</t>
+  </si>
+  <si>
+    <t>Join Table: applicants_jobs_statuses   Class: ApplicantJobStatus</t>
+  </si>
+  <si>
+    <t>Table: statuses  Class: Status</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>Senior Technical Consultant</t>
+  </si>
+  <si>
+    <t>Senior Sales Executive</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Senior Java Developer</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>Broomfield</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Patty Laushman</t>
+  </si>
+  <si>
+    <t>Jen Smith</t>
+  </si>
+  <si>
+    <t>plaushman@gmail.com</t>
+  </si>
+  <si>
+    <t>john@doe.com</t>
+  </si>
+  <si>
+    <t>jensmith@gmail.com</t>
+  </si>
+  <si>
+    <t>720-629-4538</t>
+  </si>
+  <si>
+    <t>303-123-4567</t>
+  </si>
+  <si>
+    <t>303-987-6543</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +220,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,10 +271,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -220,11 +292,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -235,105 +311,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="295275" y="628650"/>
-          <a:ext cx="5848350" cy="485775"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="285750" y="1571625"/>
-          <a:ext cx="6591300" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,23 +615,34 @@
     <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
     <col min="10" max="10" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="2"/>
+    <col min="11" max="43" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="F1" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="4"/>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -669,255 +657,369 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="2">
+        <v>80021</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2">
+        <v>80021</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="2">
+        <v>6</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="2">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <v>8</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>11</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="J23" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="J24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
         <v>14</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="J25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="2">
         <v>15</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="J26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="2">
         <v>16</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>5</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>11</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>12</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>14</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>15</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>16</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1"/>
+    <hyperlink ref="K5" r:id="rId2"/>
+    <hyperlink ref="K6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>